<commit_message>
used Autofill and Flash Fill to clean Data
</commit_message>
<xml_diff>
--- a/Exercise.xlsx
+++ b/Exercise.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78704F-621C-4427-A260-5DC5D725E3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECF44D0-33AA-4DED-A38D-5020B1CBCD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16690" yWindow="-320" windowWidth="19420" windowHeight="11020" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>Full Name</t>
   </si>
@@ -54,9 +56,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>Full Year</t>
-  </si>
-  <si>
     <t>Chante Devlin</t>
   </si>
   <si>
@@ -85,6 +84,189 @@
   </si>
   <si>
     <t>Kelsi Rich</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Office Type</t>
+  </si>
+  <si>
+    <t>Revenues</t>
+  </si>
+  <si>
+    <t>Operating Expenses</t>
+  </si>
+  <si>
+    <t>Operating Profit</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>Scorecard</t>
+  </si>
+  <si>
+    <t>Warner, NH</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Average Revenue</t>
+  </si>
+  <si>
+    <t>East Natchitoches, RI</t>
+  </si>
+  <si>
+    <t>Franchise</t>
+  </si>
+  <si>
+    <t>Highest Revenue</t>
+  </si>
+  <si>
+    <t>Lyon, MA</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Lowest Expenses</t>
+  </si>
+  <si>
+    <t>Willow Run, NH</t>
+  </si>
+  <si>
+    <t>Conyersville, RI</t>
+  </si>
+  <si>
+    <t>Mount Baker, NY</t>
+  </si>
+  <si>
+    <t>Farmington Lake, RI</t>
+  </si>
+  <si>
+    <t>Martins Corner, NH</t>
+  </si>
+  <si>
+    <t>Pickerel Narrows, ME</t>
+  </si>
+  <si>
+    <t>Willaha, NY</t>
+  </si>
+  <si>
+    <t>Center, MA</t>
+  </si>
+  <si>
+    <t>Spring City, MA</t>
+  </si>
+  <si>
+    <t>Mittenlane, NY</t>
+  </si>
+  <si>
+    <t>East Waterford, ME</t>
+  </si>
+  <si>
+    <t>Coltman, RI</t>
+  </si>
+  <si>
+    <t>Scottsville, NJ</t>
+  </si>
+  <si>
+    <t>Hebron, NH</t>
+  </si>
+  <si>
+    <t>Longview, MA</t>
+  </si>
+  <si>
+    <t>Emerson, NJ</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>City and State</t>
+  </si>
+  <si>
+    <t>Warner</t>
+  </si>
+  <si>
+    <t>East Natchitoches</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>Willow Run</t>
+  </si>
+  <si>
+    <t>Conyersville</t>
+  </si>
+  <si>
+    <t>Mount Baker</t>
+  </si>
+  <si>
+    <t>Farmington Lake</t>
+  </si>
+  <si>
+    <t>Martins Corner</t>
+  </si>
+  <si>
+    <t>Pickerel Narrows</t>
+  </si>
+  <si>
+    <t>Willaha</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>Spring City</t>
+  </si>
+  <si>
+    <t>Mittenlane</t>
+  </si>
+  <si>
+    <t>East Waterford</t>
+  </si>
+  <si>
+    <t>Coltman</t>
+  </si>
+  <si>
+    <t>Scottsville</t>
+  </si>
+  <si>
+    <t>Hebron</t>
+  </si>
+  <si>
+    <t>Longview</t>
+  </si>
+  <si>
+    <t>Emerson</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>NJ</t>
   </si>
 </sst>
 </file>
@@ -94,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +288,13 @@
       <b/>
       <sz val="14"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,13 +320,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +647,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,15 +678,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="3">
         <v>275702</v>
@@ -515,10 +707,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="3">
         <v>222562</v>
@@ -539,10 +731,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>211070</v>
@@ -563,10 +755,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3">
         <v>163774</v>
@@ -587,10 +779,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>344044</v>
@@ -611,10 +803,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>324035</v>
@@ -631,6 +823,726 @@
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>1282640</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D64E18-04DF-4C91-A84C-5EB5EC653CDA}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>125319</v>
+      </c>
+      <c r="F2">
+        <v>65792</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>59527</v>
+      </c>
+      <c r="H2">
+        <v>4667</v>
+      </c>
+      <c r="I2">
+        <f>G2-H2</f>
+        <v>54860</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(E2:E20)</f>
+        <v>276986.5263157895</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>433924</v>
+      </c>
+      <c r="F3">
+        <v>101465</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G20" si="0">E3-F3</f>
+        <v>332459</v>
+      </c>
+      <c r="H3">
+        <v>5068</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I20" si="1">G3-H3</f>
+        <v>327391</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3">
+        <f>MAX(E2:E20)</f>
+        <v>461214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>135816</v>
+      </c>
+      <c r="F4">
+        <v>67388</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>68428</v>
+      </c>
+      <c r="H4">
+        <v>5700</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>62728</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4">
+        <f>MIN(E2:E20)</f>
+        <v>125319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>233255</v>
+      </c>
+      <c r="F5">
+        <v>83606</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>149649</v>
+      </c>
+      <c r="H5">
+        <v>5089</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>144560</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>128691</v>
+      </c>
+      <c r="F6">
+        <v>67175</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>61516</v>
+      </c>
+      <c r="H6">
+        <v>4956</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>56560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>244913</v>
+      </c>
+      <c r="F7">
+        <v>89974</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>154939</v>
+      </c>
+      <c r="H7">
+        <v>5062</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>149877</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>392518</v>
+      </c>
+      <c r="F8">
+        <v>82675</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>309843</v>
+      </c>
+      <c r="H8">
+        <v>6100</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>303743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>331773</v>
+      </c>
+      <c r="F9">
+        <v>85288</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>246485</v>
+      </c>
+      <c r="H9">
+        <v>5795</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>240690</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>244975</v>
+      </c>
+      <c r="F10">
+        <v>100834</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>144141</v>
+      </c>
+      <c r="H10">
+        <v>5153</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>138988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>137925</v>
+      </c>
+      <c r="F11">
+        <v>104528</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>33397</v>
+      </c>
+      <c r="H11">
+        <v>5673</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>27724</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>207163</v>
+      </c>
+      <c r="F12">
+        <v>73705</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>133458</v>
+      </c>
+      <c r="H12">
+        <v>5599</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>127859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>432326</v>
+      </c>
+      <c r="F13">
+        <v>79297</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>353029</v>
+      </c>
+      <c r="H13">
+        <v>4872</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>348157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>177789</v>
+      </c>
+      <c r="F14">
+        <v>103757</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>74032</v>
+      </c>
+      <c r="H14">
+        <v>5144</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>68888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>201945</v>
+      </c>
+      <c r="F15">
+        <v>83178</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>118767</v>
+      </c>
+      <c r="H15">
+        <v>4734</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>114033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>461214</v>
+      </c>
+      <c r="F16">
+        <v>86688</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>374526</v>
+      </c>
+      <c r="H16">
+        <v>6066</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>368460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>440462</v>
+      </c>
+      <c r="F17">
+        <v>81912</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>358550</v>
+      </c>
+      <c r="H17">
+        <v>4842</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>353708</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>407339</v>
+      </c>
+      <c r="F18">
+        <v>88286</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>319053</v>
+      </c>
+      <c r="H18">
+        <v>4604</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>314449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>376263</v>
+      </c>
+      <c r="F19">
+        <v>92698</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>283565</v>
+      </c>
+      <c r="H19">
+        <v>5195</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>278370</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>149134</v>
+      </c>
+      <c r="F20">
+        <v>87513</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>61621</v>
+      </c>
+      <c r="H20">
+        <v>5168</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>56453</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F40AB-1F15-4573-AC0C-90024DE33C6E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>276986.5263157895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>461214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>125319</v>
       </c>
     </row>
   </sheetData>
@@ -856,18 +1768,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,18 +1802,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Autofit column width , delete the column , merge and center text
</commit_message>
<xml_diff>
--- a/Exercise.xlsx
+++ b/Exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECF44D0-33AA-4DED-A38D-5020B1CBCD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285723-7560-4DD8-93E6-938CDE8F2472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16690" yWindow="-320" windowWidth="19420" windowHeight="11020" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>Full Name</t>
   </si>
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -329,6 +329,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,9 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2969A0-E328-41DF-8FAC-1B10B2F7DEC8}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -835,54 +836,53 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J1" s="4"/>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -913,13 +913,6 @@
       <c r="I2">
         <f>G2-H2</f>
         <v>54860</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2">
-        <f>AVERAGE(E2:E20)</f>
-        <v>276986.5263157895</v>
       </c>
       <c r="N2" s="4"/>
       <c r="P2" s="4"/>
@@ -958,13 +951,6 @@
         <f t="shared" ref="I3:I20" si="1">G3-H3</f>
         <v>327391</v>
       </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3">
-        <f>MAX(E2:E20)</f>
-        <v>461214</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -995,13 +981,6 @@
       <c r="I4">
         <f t="shared" si="1"/>
         <v>62728</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4">
-        <f>MIN(E2:E20)</f>
-        <v>125319</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1508,49 +1487,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F40AB-1F15-4573-AC0C-90024DE33C6E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>276986.5263157895</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>461214</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>125319</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -1767,22 +1768,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA3212C-9EA0-4F60-9BC2-AD5EAEF2279B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1799,21 +1802,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
formatting text - header rows and a title
</commit_message>
<xml_diff>
--- a/Exercise.xlsx
+++ b/Exercise.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285723-7560-4DD8-93E6-938CDE8F2472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088A4C3-3425-4674-9649-6B28A37E154E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16690" yWindow="-320" windowWidth="19420" windowHeight="11020" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Original Dataset" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
   <si>
     <t>Full Name</t>
   </si>
@@ -267,6 +268,9 @@
   </si>
   <si>
     <t>NJ</t>
+  </si>
+  <si>
+    <t>Full Year</t>
   </si>
 </sst>
 </file>
@@ -320,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -329,9 +333,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,10 +647,555 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1DC30F-03E5-4845-92EF-BCFF78A27010}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>125319</v>
+      </c>
+      <c r="F2">
+        <v>65792</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>59527</v>
+      </c>
+      <c r="H2">
+        <v>4667</v>
+      </c>
+      <c r="I2">
+        <f>G2-H2</f>
+        <v>54860</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>275702</v>
+      </c>
+      <c r="M2">
+        <v>261290</v>
+      </c>
+      <c r="N2">
+        <v>332449</v>
+      </c>
+      <c r="O2">
+        <v>282904</v>
+      </c>
+      <c r="P2">
+        <v>1152345</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2">
+        <f>AVERAGE(E2:E20)</f>
+        <v>276986.5263157895</v>
+      </c>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>433924</v>
+      </c>
+      <c r="F3">
+        <v>101465</v>
+      </c>
+      <c r="H3">
+        <v>5068</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>222562</v>
+      </c>
+      <c r="M3">
+        <v>227580</v>
+      </c>
+      <c r="N3">
+        <v>291259</v>
+      </c>
+      <c r="O3">
+        <v>408463</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3">
+        <f>MAX(E2:E20)</f>
+        <v>461214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>135816</v>
+      </c>
+      <c r="F4">
+        <v>67388</v>
+      </c>
+      <c r="H4">
+        <v>5700</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>211070</v>
+      </c>
+      <c r="M4">
+        <v>203426</v>
+      </c>
+      <c r="N4">
+        <v>194457</v>
+      </c>
+      <c r="O4">
+        <v>358982</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4">
+        <f>MIN(E2:E20)</f>
+        <v>125319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>233255</v>
+      </c>
+      <c r="F5">
+        <v>83606</v>
+      </c>
+      <c r="H5">
+        <v>5089</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>163774</v>
+      </c>
+      <c r="M5">
+        <v>390208</v>
+      </c>
+      <c r="N5">
+        <v>315982</v>
+      </c>
+      <c r="O5">
+        <v>347702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>128691</v>
+      </c>
+      <c r="F6">
+        <v>67175</v>
+      </c>
+      <c r="H6">
+        <v>4956</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <v>344044</v>
+      </c>
+      <c r="M6">
+        <v>400640</v>
+      </c>
+      <c r="N6">
+        <v>180535</v>
+      </c>
+      <c r="O6">
+        <v>372475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>244913</v>
+      </c>
+      <c r="F7">
+        <v>89974</v>
+      </c>
+      <c r="H7">
+        <v>5062</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>324035</v>
+      </c>
+      <c r="M7">
+        <v>370979</v>
+      </c>
+      <c r="N7">
+        <v>356277</v>
+      </c>
+      <c r="O7">
+        <v>231349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>392518</v>
+      </c>
+      <c r="F8">
+        <v>82675</v>
+      </c>
+      <c r="H8">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>331773</v>
+      </c>
+      <c r="F9">
+        <v>85288</v>
+      </c>
+      <c r="H9">
+        <v>5795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>244975</v>
+      </c>
+      <c r="F10">
+        <v>100834</v>
+      </c>
+      <c r="H10">
+        <v>5153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>137925</v>
+      </c>
+      <c r="F11">
+        <v>104528</v>
+      </c>
+      <c r="H11">
+        <v>5673</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>207163</v>
+      </c>
+      <c r="F12">
+        <v>73705</v>
+      </c>
+      <c r="H12">
+        <v>5599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>432326</v>
+      </c>
+      <c r="F13">
+        <v>79297</v>
+      </c>
+      <c r="H13">
+        <v>4872</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>177789</v>
+      </c>
+      <c r="F14">
+        <v>103757</v>
+      </c>
+      <c r="H14">
+        <v>5144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>201945</v>
+      </c>
+      <c r="F15">
+        <v>83178</v>
+      </c>
+      <c r="H15">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>461214</v>
+      </c>
+      <c r="F16">
+        <v>86688</v>
+      </c>
+      <c r="H16">
+        <v>6066</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>440462</v>
+      </c>
+      <c r="F17">
+        <v>81912</v>
+      </c>
+      <c r="H17">
+        <v>4842</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>407339</v>
+      </c>
+      <c r="F18">
+        <v>88286</v>
+      </c>
+      <c r="H18">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>376263</v>
+      </c>
+      <c r="F19">
+        <v>92698</v>
+      </c>
+      <c r="H19">
+        <v>5195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>149134</v>
+      </c>
+      <c r="F20">
+        <v>87513</v>
+      </c>
+      <c r="H20">
+        <v>5168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2969A0-E328-41DF-8FAC-1B10B2F7DEC8}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -831,12 +1377,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D64E18-04DF-4C91-A84C-5EB5EC653CDA}">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,12 +2031,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F40AB-1F15-4573-AC0C-90024DE33C6E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,11 +2044,11 @@
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1529,29 +2075,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -1768,24 +2296,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA3212C-9EA0-4F60-9BC2-AD5EAEF2279B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1802,4 +2328,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Borders , fills , regional number formatting
</commit_message>
<xml_diff>
--- a/Exercise.xlsx
+++ b/Exercise.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9088A4C3-3425-4674-9649-6B28A37E154E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3062D9-5489-431B-AB3E-76B14D4E05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16690" yWindow="-320" windowWidth="19420" windowHeight="11020" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
+    <workbookView xWindow="16690" yWindow="-320" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{A7F1AEE3-0EAD-4639-A56C-8AAFF0B9C8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dataset" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Financial Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Financial Scorecard" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -277,8 +277,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -304,15 +305,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -320,11 +327,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -334,6 +350,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1DC30F-03E5-4845-92EF-BCFF78A27010}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1382,7 +1400,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,32 +1418,32 @@
     <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J1" s="4"/>
@@ -1443,20 +1461,20 @@
       <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>125319</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>65792</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <f>E2-F2</f>
         <v>59527</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>4667</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <f>G2-H2</f>
         <v>54860</v>
       </c>
@@ -1480,20 +1498,20 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>433924</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>101465</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G20" si="0">E3-F3</f>
         <v>332459</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>5068</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <f t="shared" ref="I3:I20" si="1">G3-H3</f>
         <v>327391</v>
       </c>
@@ -1511,20 +1529,20 @@
       <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>135816</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>67388</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <f t="shared" si="0"/>
         <v>68428</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>5700</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <f t="shared" si="1"/>
         <v>62728</v>
       </c>
@@ -1542,20 +1560,20 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>233255</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>83606</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>149649</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>5089</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <f t="shared" si="1"/>
         <v>144560</v>
       </c>
@@ -1574,20 +1592,20 @@
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>128691</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>67175</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>61516</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>4956</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <f t="shared" si="1"/>
         <v>56560</v>
       </c>
@@ -1605,20 +1623,20 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>244913</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>89974</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>154939</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>5062</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <f t="shared" si="1"/>
         <v>149877</v>
       </c>
@@ -1636,20 +1654,20 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>392518</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>82675</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>309843</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>6100</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <f t="shared" si="1"/>
         <v>303743</v>
       </c>
@@ -1667,20 +1685,20 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>331773</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>85288</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>246485</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>5795</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <f t="shared" si="1"/>
         <v>240690</v>
       </c>
@@ -1698,20 +1716,20 @@
       <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>244975</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>100834</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>144141</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>5153</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <f t="shared" si="1"/>
         <v>138988</v>
       </c>
@@ -1729,20 +1747,20 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>137925</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>104528</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>33397</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>5673</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <f t="shared" si="1"/>
         <v>27724</v>
       </c>
@@ -1760,20 +1778,20 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>207163</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>73705</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>133458</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>5599</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <f t="shared" si="1"/>
         <v>127859</v>
       </c>
@@ -1791,20 +1809,20 @@
       <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>432326</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>79297</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>353029</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>4872</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <f t="shared" si="1"/>
         <v>348157</v>
       </c>
@@ -1822,20 +1840,20 @@
       <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>177789</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>103757</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>74032</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>5144</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <f t="shared" si="1"/>
         <v>68888</v>
       </c>
@@ -1853,20 +1871,20 @@
       <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>201945</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <v>83178</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>118767</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>4734</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <f t="shared" si="1"/>
         <v>114033</v>
       </c>
@@ -1884,20 +1902,20 @@
       <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>461214</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <v>86688</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>374526</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>6066</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="5">
         <f t="shared" si="1"/>
         <v>368460</v>
       </c>
@@ -1915,20 +1933,20 @@
       <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>440462</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="5">
         <v>81912</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>358550</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>4842</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="5">
         <f t="shared" si="1"/>
         <v>353708</v>
       </c>
@@ -1946,20 +1964,20 @@
       <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>407339</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="5">
         <v>88286</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>319053</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>4604</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <f t="shared" si="1"/>
         <v>314449</v>
       </c>
@@ -1977,20 +1995,20 @@
       <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>376263</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="5">
         <v>92698</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>283565</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>5195</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <f t="shared" si="1"/>
         <v>278370</v>
       </c>
@@ -2008,20 +2026,20 @@
       <c r="D20" t="s">
         <v>29</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>149134</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <v>87513</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>61621</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>5168</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <f t="shared" si="1"/>
         <v>56453</v>
       </c>
@@ -2035,13 +2053,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F40AB-1F15-4573-AC0C-90024DE33C6E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2054,7 +2073,7 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>276986.5263157895</v>
       </c>
     </row>
@@ -2062,7 +2081,7 @@
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>461214</v>
       </c>
     </row>
@@ -2070,7 +2089,7 @@
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>125319</v>
       </c>
     </row>
@@ -2080,6 +2099,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -2296,22 +2330,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA3212C-9EA0-4F60-9BC2-AD5EAEF2279B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2328,21 +2364,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16C85F02-9775-4D6C-AF6B-784E84E858E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5A85AC-2CBD-412F-82B1-8F6832D6B804}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>